<commit_message>
Added new expression-related and drug-related evidence codes. These will appear in ECO soon.
</commit_message>
<xml_diff>
--- a/cttv_evidence_codes.xlsx
+++ b/cttv_evidence_codes.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="cttv_evidence_codes" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="168">
   <si>
     <t>Category</t>
   </si>
@@ -190,12 +191,6 @@
     <t>Therapeutic</t>
   </si>
   <si>
-    <t>Gene-Disease association via Drug</t>
-  </si>
-  <si>
-    <t>ECO_DRUG_NEW</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -220,281 +215,317 @@
     <t>ECO_0000010</t>
   </si>
   <si>
+    <t>transcript expression evidence</t>
+  </si>
+  <si>
+    <t>ECO_0000009</t>
+  </si>
+  <si>
+    <t>expression pattern evidence</t>
+  </si>
+  <si>
+    <t>Experimental evidence that is based on characterization of gene expression.</t>
+  </si>
+  <si>
+    <t>ECO_0000008</t>
+  </si>
+  <si>
+    <t>expression microarray evidence</t>
+  </si>
+  <si>
+    <t>ECO_0000058</t>
+  </si>
+  <si>
+    <t>baseline expression evidence</t>
+  </si>
+  <si>
+    <t>Doesn't exist yet</t>
+  </si>
+  <si>
+    <t>differential expression evidence</t>
+  </si>
+  <si>
+    <t>ECO_DIFF_EXPRESS_ROOT</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>transcript expression evidence</t>
-  </si>
-  <si>
-    <t>ECO_0000009</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>expression pattern evidence</t>
-  </si>
-  <si>
-    <t>Experimental evidence that is based on characterization of gene expression.</t>
-  </si>
-  <si>
-    <t>ECO_0000008</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>expression microarray evidence</t>
-  </si>
-  <si>
-    <t>ECO_0000058</t>
-  </si>
-  <si>
-    <t>baseline expression evidence</t>
-  </si>
-  <si>
-    <t>Doesn't exist yet</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>differential expression evidence</t>
-  </si>
-  <si>
-    <t>ECO_DIFF_EXPRESS_ROOT</t>
+    <t>genomic microarray evidence</t>
+  </si>
+  <si>
+    <t>ECO_0000062</t>
+  </si>
+  <si>
+    <t>induced mutation evidence</t>
+  </si>
+  <si>
+    <t>ECO_0001056</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>computational combinatorial evidence</t>
+  </si>
+  <si>
+    <t>A type of combinatorial analysis where data are combined and evaluated by an algorithm.</t>
+  </si>
+  <si>
+    <t>ECO_0000053</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>differential gene expression from microarray experiments</t>
-  </si>
-  <si>
-    <t>ECO_DIFF_EXPRESS_MICROARRAY_NEW</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>differential gene expression from RNA-seq experiments</t>
-  </si>
-  <si>
-    <t>ECO_DIFF_RNASEQ_NEW</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>differential geneset expression from microarray experiments (GSEA, Fisher-exact)</t>
-  </si>
-  <si>
-    <t>ECO_DIFF_GENESET_MICROARRAY_NEW</t>
+    <t>constitutively active mutant evidence</t>
+  </si>
+  <si>
+    <t>ECO_0001032</t>
+  </si>
+  <si>
+    <t>medical imaging evidence</t>
+  </si>
+  <si>
+    <t>ECO_0001097</t>
+  </si>
+  <si>
+    <t>mutant phenotype evidence</t>
+  </si>
+  <si>
+    <t>The IMP evidence code covers those cases when the function, process or cellular localization of a gene product is inferred based on differences in the function, process, or cellular localization between two different alleles of the corresponding gene. The IMP code is used for cases where one allele may be designated 'wild-type' and another as 'mutant'. It is also used in cases where allelic variation occurs naturally and no specific allele is designated as wild-type or mutant. Caution should be used when making annotations from gain-of-function mutations as it may be difficult to infer a gene's normal function from a gain of function mutation, although it is sometimes possible.</t>
+  </si>
+  <si>
+    <t>ECO_0000015</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>differential geneset expression from RNA-seq experiments (GSEA, Fisher-exact)</t>
-  </si>
-  <si>
-    <t>ECO_DIFF_GENESET_RNASEQ_NEW</t>
+    <t>natural variation mutant evidence</t>
+  </si>
+  <si>
+    <t>ECO_0001103</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>genomic microarray evidence</t>
-  </si>
-  <si>
-    <t>ECO_0000062</t>
-  </si>
-  <si>
-    <t>induced mutation evidence</t>
-  </si>
-  <si>
-    <t>ECO_0001056</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>computational combinatorial evidence</t>
-  </si>
-  <si>
-    <t>A type of combinatorial analysis where data are combined and evaluated by an algorithm.</t>
-  </si>
-  <si>
-    <t>ECO_0000053</t>
+    <t>phylogenetic determination of loss of key residues evidence</t>
+  </si>
+  <si>
+    <t>A type of phylogenetic evidence characterized by the absence of key sequence residues.</t>
+  </si>
+  <si>
+    <t>ECO_0000216</t>
+  </si>
+  <si>
+    <t>Evidence codes from Gene ontology (http://geneontology.org/)</t>
+  </si>
+  <si>
+    <t>Involvement of protein in disease (literature evidence)</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
+    <t>Related proteins (Uniref clusters)</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
+    <t>Phenotype disruption (Literature evidence)</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>constitutively active mutant evidence</t>
-  </si>
-  <si>
-    <t>ECO_0001032</t>
-  </si>
-  <si>
-    <t>medical imaging evidence</t>
-  </si>
-  <si>
-    <t>ECO_0001097</t>
-  </si>
-  <si>
-    <t>mutant phenotype evidence</t>
-  </si>
-  <si>
-    <t>The IMP evidence code covers those cases when the function, process or cellular localization of a gene product is inferred based on differences in the function, process, or cellular localization between two different alleles of the corresponding gene. The IMP code is used for cases where one allele may be designated 'wild-type' and another as 'mutant'. It is also used in cases where allelic variation occurs naturally and no specific allele is designated as wild-type or mutant. Caution should be used when making annotations from gain-of-function mutations as it may be difficult to infer a gene's normal function from a gain of function mutation, although it is sometimes possible.</t>
-  </si>
-  <si>
-    <t>ECO_0000015</t>
+    <t>Enzyme regulation (Literature evidence)</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>natural variation mutant evidence</t>
-  </si>
-  <si>
-    <t>ECO_0001103</t>
+    <t>Protein function (Literature evidence)</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>phylogenetic determination of loss of key residues evidence</t>
-  </si>
-  <si>
-    <t>A type of phylogenetic evidence characterized by the absence of key sequence residues.</t>
-  </si>
-  <si>
-    <t>ECO_0000216</t>
-  </si>
-  <si>
-    <t>Evidence codes from Gene ontology (http://geneontology.org/)</t>
-  </si>
-  <si>
-    <t>Involvement of protein in disease (literature evidence)</t>
+    <t>Variants mutagens (Expert evidence from literature)</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Related proteins (Uniref clusters)</t>
+    <t>Protein sequence (including isoforms)</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Phenotype disruption (Literature evidence)</t>
+    <t>Predictions</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Enzyme regulation (Literature evidence)</t>
+    <t>Annotated interactions</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Protein function (Literature evidence)</t>
+    <t>Protein expression</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Variants mutagens (Expert evidence from literature)</t>
+    <t>Annotated structures</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Protein sequence (including isoforms)</t>
+    <t>Curated cross references</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Predictions</t>
+    <t>Protein co-ordinates</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Annotated interactions</t>
+    <t>Subcellular location</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Protein expression</t>
+    <t>Annotated pathways</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Annotated structures</t>
+    <t>Target in specific disease</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Curated cross references</t>
+    <t>PTH</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Protein co-ordinates</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Subcellular location</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Annotated pathways</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Target in specific disease</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>PTH</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Pharma. Use of protein (Literature evidence)</t>
   </si>
   <si>
     <t>UNIPROT_MAPPING</t>
+  </si>
+  <si>
+    <t>differential gene expression from microarray experiment</t>
+  </si>
+  <si>
+    <t>differential gene expression from RNA-seq experiment</t>
+  </si>
+  <si>
+    <t>differential geneset expression from microarray experiment</t>
+  </si>
+  <si>
+    <t>differential geneset expression from RNA-seq experiment</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>ECO:0000356</t>
+  </si>
+  <si>
+    <t>differential gene expression evidence from microarray experiment</t>
+  </si>
+  <si>
+    <t>A gene is found to show statistically significant increase or decrease in expression in some condition relative to an appropriate control condition, when expression levels are assayed using a microarray platform.</t>
+  </si>
+  <si>
+    <t>ECO:0000357</t>
+  </si>
+  <si>
+    <t>differential gene expression evidence from RNA-seq experiment</t>
+  </si>
+  <si>
+    <t>A gene is found to show statistically significant increase or decrease in expression in some condition relative to an appropriate control condition, when expression levels are assayed using an RNA sequencing platform.</t>
+  </si>
+  <si>
+    <t>ECO:0000358</t>
+  </si>
+  <si>
+    <t>differential geneset expression evidence from microarray experiment</t>
+  </si>
+  <si>
+    <t>Gene set enrichment analysis (GSEA) shows that a functional classification (e.g. reaction pathway, Gene Ontology term, etc) has statistically significant over-representation in a group of genes showing differential expression when assayed using a microarray platform.</t>
+  </si>
+  <si>
+    <t>ECO:0000359</t>
+  </si>
+  <si>
+    <t>differential geneset expression evidence from RNA-seq experiment</t>
+  </si>
+  <si>
+    <t>Gene set enrichment analysis (GSEA) shows that a functional classification (e.g. reaction pathway, Gene Ontology term, etc) has statistically significant over-representation in a group of genes showing differential expression when assayed using an RNA sequencing platform.</t>
+  </si>
+  <si>
+    <t>biological target-disease association via drug</t>
+  </si>
+  <si>
+    <t>ECO_0000360</t>
+  </si>
+  <si>
+    <t>ECO_0000356</t>
+  </si>
+  <si>
+    <t>ECO_0000357</t>
+  </si>
+  <si>
+    <t>ECO_0000358</t>
+  </si>
+  <si>
+    <t>ECO_0000359</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -559,11 +590,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -724,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -787,28 +813,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -817,6 +840,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,7 +854,7 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -844,7 +874,21 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1226,44 +1270,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1308,15 +1314,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1330,6 +1327,39 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1372,11 +1402,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L53" totalsRowShown="0" headerRowDxfId="16" dataDxfId="0" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L53" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <tableColumns count="12">
-    <tableColumn id="1" name="Category" dataDxfId="12"/>
-    <tableColumn id="2" name="EvidenceLabel" dataDxfId="11"/>
-    <tableColumn id="3" name="evidence_code_description" dataDxfId="10"/>
+    <tableColumn id="1" name="Category" dataDxfId="11"/>
+    <tableColumn id="2" name="EvidenceLabel" dataDxfId="10"/>
+    <tableColumn id="3" name="evidence_code_description" dataDxfId="0"/>
     <tableColumn id="4" name="evidence_code_id" dataDxfId="9"/>
     <tableColumn id="5" name="Rare2Common (CTTV005) - James" dataDxfId="8"/>
     <tableColumn id="6" name="ChEMBL (CTTV008) - John Overington" dataDxfId="7"/>
@@ -1679,14 +1709,14 @@
   <dimension ref="A1:L1034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="56" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="33" customWidth="1"/>
     <col min="4" max="4" width="37.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="17.28515625" style="4"/>
@@ -2013,15 +2043,15 @@
         <v>57</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="21" t="s">
-        <v>59</v>
+      <c r="D15" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2032,14 +2062,14 @@
     </row>
     <row r="16" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -2053,11 +2083,11 @@
     <row r="17" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -2071,18 +2101,16 @@
     <row r="18" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="19" t="s">
-        <v>68</v>
-      </c>
+      <c r="H18" s="19"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2091,18 +2119,16 @@
     <row r="19" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="11" t="s">
-        <v>71</v>
-      </c>
+      <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -2111,20 +2137,18 @@
     <row r="20" spans="1:12" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="15" t="s">
-        <v>75</v>
-      </c>
+      <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -2133,11 +2157,11 @@
     <row r="21" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2151,18 +2175,16 @@
     <row r="22" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
@@ -2171,97 +2193,103 @@
     <row r="23" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="22" t="s">
-        <v>82</v>
+      <c r="D23" s="21" t="s">
+        <v>76</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="21" t="s">
-        <v>85</v>
+    <row r="24" spans="1:12" customFormat="1" ht="62.25" customHeight="1">
+      <c r="A24" s="22"/>
+      <c r="B24" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>164</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="16"/>
     </row>
-    <row r="25" spans="1:12" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="21" t="s">
-        <v>88</v>
+    <row r="25" spans="1:12" customFormat="1" ht="65.25" customHeight="1">
+      <c r="A25" s="22"/>
+      <c r="B25" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>165</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="16"/>
     </row>
-    <row r="26" spans="1:12" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="21" t="s">
-        <v>91</v>
+    <row r="26" spans="1:12" customFormat="1" ht="83.25" customHeight="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>166</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="19" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="16"/>
     </row>
-    <row r="27" spans="1:12" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="21" t="s">
-        <v>94</v>
+    <row r="27" spans="1:12" customFormat="1" ht="96.75" customHeight="1">
+      <c r="A27" s="22"/>
+      <c r="B27" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>167</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="19" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -2271,11 +2299,11 @@
     <row r="28" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="13"/>
       <c r="B28" s="14" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -2289,11 +2317,11 @@
     <row r="29" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="10" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -2306,16 +2334,16 @@
     </row>
     <row r="30" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -2324,24 +2352,24 @@
       </c>
       <c r="H30" s="15"/>
       <c r="I30" s="15" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="L30" s="20"/>
     </row>
     <row r="31" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="10" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -2355,11 +2383,11 @@
     <row r="32" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
@@ -2373,20 +2401,20 @@
     <row r="33" spans="1:12" customFormat="1" ht="285" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="10" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
@@ -2395,18 +2423,18 @@
     <row r="34" spans="1:12" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -2415,13 +2443,13 @@
     <row r="35" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -2433,22 +2461,22 @@
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" customFormat="1" ht="45" customHeight="1">
-      <c r="A36" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>122</v>
+      <c r="A36" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="25" t="s">
-        <v>157</v>
+      <c r="D36" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="17" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
@@ -2456,19 +2484,19 @@
     </row>
     <row r="37" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A37" s="9"/>
-      <c r="B37" s="22" t="s">
-        <v>124</v>
+      <c r="B37" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="25" t="s">
-        <v>157</v>
+      <c r="D37" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="17" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
@@ -2476,19 +2504,19 @@
     </row>
     <row r="38" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A38" s="9"/>
-      <c r="B38" s="22" t="s">
-        <v>126</v>
+      <c r="B38" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="25" t="s">
-        <v>157</v>
+      <c r="D38" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="17" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
@@ -2496,19 +2524,19 @@
     </row>
     <row r="39" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A39" s="9"/>
-      <c r="B39" s="22" t="s">
-        <v>128</v>
+      <c r="B39" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="25" t="s">
-        <v>157</v>
+      <c r="D39" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="17" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
@@ -2516,19 +2544,19 @@
     </row>
     <row r="40" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A40" s="9"/>
-      <c r="B40" s="22" t="s">
-        <v>130</v>
+      <c r="B40" s="21" t="s">
+        <v>115</v>
       </c>
       <c r="C40" s="10"/>
-      <c r="D40" s="25" t="s">
-        <v>157</v>
+      <c r="D40" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="17" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
@@ -2536,19 +2564,19 @@
     </row>
     <row r="41" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="22" t="s">
-        <v>132</v>
+      <c r="B41" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="C41" s="10"/>
-      <c r="D41" s="25" t="s">
-        <v>157</v>
+      <c r="D41" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
       <c r="I41" s="17" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
@@ -2556,19 +2584,19 @@
     </row>
     <row r="42" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="22" t="s">
-        <v>134</v>
+      <c r="B42" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="C42" s="10"/>
-      <c r="D42" s="25" t="s">
-        <v>157</v>
+      <c r="D42" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
       <c r="I42" s="17" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -2576,19 +2604,19 @@
     </row>
     <row r="43" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="22" t="s">
-        <v>136</v>
+      <c r="B43" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="C43" s="10"/>
-      <c r="D43" s="25" t="s">
-        <v>157</v>
+      <c r="D43" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="17" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
@@ -2596,19 +2624,19 @@
     </row>
     <row r="44" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="22" t="s">
-        <v>138</v>
+      <c r="B44" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="25" t="s">
-        <v>157</v>
+      <c r="D44" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="17" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -2616,19 +2644,19 @@
     </row>
     <row r="45" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="22" t="s">
-        <v>140</v>
+      <c r="B45" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="C45" s="10"/>
-      <c r="D45" s="25" t="s">
-        <v>157</v>
+      <c r="D45" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="17" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
@@ -2636,19 +2664,19 @@
     </row>
     <row r="46" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="24" t="s">
         <v>142</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="25" t="s">
-        <v>157</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="17" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -2656,19 +2684,19 @@
     </row>
     <row r="47" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="22" t="s">
-        <v>144</v>
+      <c r="B47" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="25" t="s">
-        <v>157</v>
+      <c r="D47" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="17" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
@@ -2676,19 +2704,19 @@
     </row>
     <row r="48" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="22" t="s">
-        <v>146</v>
+      <c r="B48" s="21" t="s">
+        <v>131</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="25" t="s">
-        <v>157</v>
+      <c r="D48" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="17" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -2696,19 +2724,19 @@
     </row>
     <row r="49" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="22" t="s">
-        <v>148</v>
+      <c r="B49" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="25" t="s">
-        <v>157</v>
+      <c r="D49" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="17" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
@@ -2716,19 +2744,19 @@
     </row>
     <row r="50" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="22" t="s">
-        <v>150</v>
+      <c r="B50" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="25" t="s">
-        <v>157</v>
+      <c r="D50" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="17" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
@@ -2736,19 +2764,19 @@
     </row>
     <row r="51" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="22" t="s">
-        <v>152</v>
+      <c r="B51" s="21" t="s">
+        <v>137</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="25" t="s">
-        <v>157</v>
+      <c r="D51" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="17" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
@@ -2756,41 +2784,41 @@
     </row>
     <row r="52" spans="1:12" customFormat="1" ht="45" customHeight="1">
       <c r="A52" s="9"/>
-      <c r="B52" s="22" t="s">
-        <v>154</v>
+      <c r="B52" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="25" t="s">
-        <v>157</v>
+      <c r="D52" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="17" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="12"/>
     </row>
     <row r="53" spans="1:12" customFormat="1" ht="45" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="31"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="30"/>
     </row>
     <row r="54" spans="1:12" ht="45" customHeight="1">
       <c r="A54" s="1"/>
@@ -16533,4 +16561,78 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a new column showing whether ECO codes were added recently.
Signed-off-by: Samiul Hasan <shasan77@gmail.com>
</commit_message>
<xml_diff>
--- a/cttv_evidence_codes.xlsx
+++ b/cttv_evidence_codes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
   <si>
     <t>Category</t>
   </si>
@@ -445,6 +445,12 @@
   <si>
     <t>Biotechnology use</t>
   </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>ECO status</t>
+  </si>
 </sst>
 </file>
 
@@ -701,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -824,11 +830,38 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1379,27 +1412,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L53" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A1:L53">
-    <filterColumn colId="9">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M53" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:M53">
+    <filterColumn colId="9"/>
+    <filterColumn colId="12"/>
   </autoFilter>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Category" dataDxfId="11"/>
-    <tableColumn id="2" name="EvidenceLabel" dataDxfId="10"/>
-    <tableColumn id="3" name="evidence_code_description" dataDxfId="9"/>
-    <tableColumn id="4" name="evidence_code_id" dataDxfId="8"/>
-    <tableColumn id="5" name="Rare2Common (CTTV005) - James" dataDxfId="7"/>
-    <tableColumn id="6" name="ChEMBL (CTTV008) - John Overington" dataDxfId="6"/>
-    <tableColumn id="7" name="GWAS (CTTV009) - Tony" dataDxfId="5"/>
-    <tableColumn id="8" name="Tissue (specificity (CTTV010) - Robert" dataDxfId="4"/>
-    <tableColumn id="9" name="Uniprot (CTTV011) - Claire" dataDxfId="3"/>
-    <tableColumn id="10" name="Variation (CTTV012) - Justin" dataDxfId="2"/>
-    <tableColumn id="11" name="IBD_GWAS (CTTV018) - Sarah" dataDxfId="1"/>
-    <tableColumn id="12" name="Networks (CTTV006) - Sandra" dataDxfId="0"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Category" dataDxfId="12"/>
+    <tableColumn id="2" name="EvidenceLabel" dataDxfId="11"/>
+    <tableColumn id="3" name="evidence_code_description" dataDxfId="10"/>
+    <tableColumn id="4" name="evidence_code_id" dataDxfId="9"/>
+    <tableColumn id="5" name="Rare2Common (CTTV005) - James" dataDxfId="8"/>
+    <tableColumn id="6" name="ChEMBL (CTTV008) - John Overington" dataDxfId="7"/>
+    <tableColumn id="7" name="GWAS (CTTV009) - Tony" dataDxfId="6"/>
+    <tableColumn id="8" name="Tissue (specificity (CTTV010) - Robert" dataDxfId="5"/>
+    <tableColumn id="9" name="Uniprot (CTTV011) - Claire" dataDxfId="4"/>
+    <tableColumn id="10" name="Variation (CTTV012) - Justin" dataDxfId="3"/>
+    <tableColumn id="11" name="IBD_GWAS (CTTV018) - Sarah" dataDxfId="2"/>
+    <tableColumn id="12" name="Networks (CTTV006) - Sandra" dataDxfId="1"/>
+    <tableColumn id="13" name="ECO status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1690,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1034"/>
+  <dimension ref="A1:M1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1709,7 +1740,7 @@
     <col min="13" max="16384" width="17.28515625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customFormat="1" ht="228" customHeight="1">
+    <row r="1" spans="1:13" customFormat="1" ht="228" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +1777,11 @@
       <c r="L1" s="38" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M1" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1766,8 +1800,9 @@
       <c r="J2" s="40"/>
       <c r="K2" s="9"/>
       <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M2" s="44"/>
+    </row>
+    <row r="3" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>15</v>
@@ -1784,8 +1819,9 @@
       <c r="J3" s="40"/>
       <c r="K3" s="13"/>
       <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M3" s="44"/>
+    </row>
+    <row r="4" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>17</v>
@@ -1802,8 +1838,9 @@
       <c r="J4" s="40"/>
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M4" s="44"/>
+    </row>
+    <row r="5" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>19</v>
@@ -1822,8 +1859,9 @@
       <c r="J5" s="40"/>
       <c r="K5" s="13"/>
       <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M5" s="44"/>
+    </row>
+    <row r="6" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
         <v>22</v>
@@ -1840,8 +1878,9 @@
       <c r="J6" s="40"/>
       <c r="K6" s="9"/>
       <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="M6" s="44"/>
+    </row>
+    <row r="7" spans="1:13" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="12" t="s">
         <v>24</v>
@@ -1860,8 +1899,9 @@
       <c r="J7" s="40"/>
       <c r="K7" s="13"/>
       <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" customFormat="1" ht="45" customHeight="1">
+      <c r="M7" s="44"/>
+    </row>
+    <row r="8" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
         <v>27</v>
@@ -1886,8 +1926,9 @@
         <v>31</v>
       </c>
       <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" customFormat="1" ht="15" customHeight="1">
+      <c r="M8" s="44"/>
+    </row>
+    <row r="9" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
         <v>32</v>
@@ -1910,8 +1951,9 @@
         <v>34</v>
       </c>
       <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="1:12" customFormat="1" ht="30" customHeight="1">
+      <c r="M9" s="44"/>
+    </row>
+    <row r="10" spans="1:13" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
@@ -1940,8 +1982,9 @@
       <c r="L10" s="16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" customFormat="1" ht="60" hidden="1" customHeight="1">
+      <c r="M10" s="44"/>
+    </row>
+    <row r="11" spans="1:13" customFormat="1" ht="60" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>41</v>
@@ -1962,8 +2005,9 @@
       <c r="L11" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="M11" s="44"/>
+    </row>
+    <row r="12" spans="1:13" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
         <v>45</v>
@@ -1982,8 +2026,9 @@
       <c r="J12" s="40"/>
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M12" s="44"/>
+    </row>
+    <row r="13" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
         <v>48</v>
@@ -2002,8 +2047,9 @@
       <c r="J13" s="40"/>
       <c r="K13" s="13"/>
       <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M13" s="44"/>
+    </row>
+    <row r="14" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>51</v>
       </c>
@@ -2024,8 +2070,9 @@
       <c r="J14" s="40"/>
       <c r="K14" s="9"/>
       <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M14" s="44"/>
+    </row>
+    <row r="15" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>55</v>
       </c>
@@ -2046,8 +2093,11 @@
       <c r="J15" s="40"/>
       <c r="K15" s="13"/>
       <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M15" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>57</v>
       </c>
@@ -2066,8 +2116,9 @@
       <c r="J16" s="40"/>
       <c r="K16" s="13"/>
       <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M16" s="44"/>
+    </row>
+    <row r="17" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="8" t="s">
         <v>60</v>
@@ -2084,8 +2135,9 @@
       <c r="J17" s="40"/>
       <c r="K17" s="9"/>
       <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M17" s="44"/>
+    </row>
+    <row r="18" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
         <v>62</v>
@@ -2102,8 +2154,9 @@
       <c r="J18" s="40"/>
       <c r="K18" s="13"/>
       <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M18" s="44"/>
+    </row>
+    <row r="19" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="8" t="s">
         <v>64</v>
@@ -2120,8 +2173,9 @@
       <c r="J19" s="40"/>
       <c r="K19" s="9"/>
       <c r="L19" s="10"/>
-    </row>
-    <row r="20" spans="1:12" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="M19" s="44"/>
+    </row>
+    <row r="20" spans="1:13" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="12" t="s">
         <v>66</v>
@@ -2140,8 +2194,9 @@
       <c r="J20" s="40"/>
       <c r="K20" s="13"/>
       <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M20" s="44"/>
+    </row>
+    <row r="21" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="8" t="s">
         <v>69</v>
@@ -2158,8 +2213,9 @@
       <c r="J21" s="40"/>
       <c r="K21" s="9"/>
       <c r="L21" s="10"/>
-    </row>
-    <row r="22" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M21" s="44"/>
+    </row>
+    <row r="22" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
         <v>71</v>
@@ -2176,8 +2232,9 @@
       <c r="J22" s="40"/>
       <c r="K22" s="13"/>
       <c r="L22" s="14"/>
-    </row>
-    <row r="23" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M22" s="44"/>
+    </row>
+    <row r="23" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
         <v>73</v>
@@ -2194,8 +2251,9 @@
       <c r="J23" s="40"/>
       <c r="K23" s="9"/>
       <c r="L23" s="10"/>
-    </row>
-    <row r="24" spans="1:12" customFormat="1" ht="62.25" hidden="1" customHeight="1">
+      <c r="M23" s="44"/>
+    </row>
+    <row r="24" spans="1:13" customFormat="1" ht="62.25" customHeight="1">
       <c r="A24" s="20"/>
       <c r="B24" s="8" t="s">
         <v>116</v>
@@ -2216,8 +2274,11 @@
       <c r="J24" s="40"/>
       <c r="K24" s="13"/>
       <c r="L24" s="14"/>
-    </row>
-    <row r="25" spans="1:12" customFormat="1" ht="65.25" hidden="1" customHeight="1">
+      <c r="M24" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" customFormat="1" ht="65.25" customHeight="1">
       <c r="A25" s="20"/>
       <c r="B25" s="8" t="s">
         <v>117</v>
@@ -2238,8 +2299,11 @@
       <c r="J25" s="40"/>
       <c r="K25" s="13"/>
       <c r="L25" s="14"/>
-    </row>
-    <row r="26" spans="1:12" customFormat="1" ht="83.25" hidden="1" customHeight="1">
+      <c r="M25" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" customFormat="1" ht="83.25" customHeight="1">
       <c r="A26" s="20"/>
       <c r="B26" s="8" t="s">
         <v>118</v>
@@ -2260,8 +2324,11 @@
       <c r="J26" s="40"/>
       <c r="K26" s="13"/>
       <c r="L26" s="14"/>
-    </row>
-    <row r="27" spans="1:12" customFormat="1" ht="96.75" hidden="1" customHeight="1">
+      <c r="M26" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" customFormat="1" ht="96.75" customHeight="1">
       <c r="A27" s="20"/>
       <c r="B27" s="8" t="s">
         <v>119</v>
@@ -2282,8 +2349,11 @@
       <c r="J27" s="40"/>
       <c r="K27" s="13"/>
       <c r="L27" s="14"/>
-    </row>
-    <row r="28" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M27" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
         <v>79</v>
@@ -2300,8 +2370,9 @@
       <c r="J28" s="40"/>
       <c r="K28" s="13"/>
       <c r="L28" s="14"/>
-    </row>
-    <row r="29" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M28" s="44"/>
+    </row>
+    <row r="29" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="8" t="s">
         <v>81</v>
@@ -2318,8 +2389,9 @@
       <c r="J29" s="40"/>
       <c r="K29" s="9"/>
       <c r="L29" s="10"/>
-    </row>
-    <row r="30" spans="1:12" customFormat="1" ht="45" customHeight="1">
+      <c r="M29" s="44"/>
+    </row>
+    <row r="30" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A30" s="11" t="s">
         <v>83</v>
       </c>
@@ -2348,8 +2420,9 @@
         <v>87</v>
       </c>
       <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M30" s="44"/>
+    </row>
+    <row r="31" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="8" t="s">
         <v>88</v>
@@ -2366,8 +2439,9 @@
       <c r="J31" s="40"/>
       <c r="K31" s="9"/>
       <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M31" s="44"/>
+    </row>
+    <row r="32" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="11"/>
       <c r="B32" s="12" t="s">
         <v>90</v>
@@ -2384,8 +2458,9 @@
       <c r="J32" s="40"/>
       <c r="K32" s="13"/>
       <c r="L32" s="14"/>
-    </row>
-    <row r="33" spans="1:12" customFormat="1" ht="285" hidden="1" customHeight="1">
+      <c r="M32" s="44"/>
+    </row>
+    <row r="33" spans="1:13" customFormat="1" ht="285" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
         <v>92</v>
@@ -2406,8 +2481,9 @@
       <c r="J33" s="40"/>
       <c r="K33" s="9"/>
       <c r="L33" s="10"/>
-    </row>
-    <row r="34" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="M33" s="44"/>
+    </row>
+    <row r="34" spans="1:13" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="11"/>
       <c r="B34" s="12" t="s">
         <v>95</v>
@@ -2426,8 +2502,9 @@
       <c r="J34" s="40"/>
       <c r="K34" s="13"/>
       <c r="L34" s="14"/>
-    </row>
-    <row r="35" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M34" s="44"/>
+    </row>
+    <row r="35" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
         <v>97</v>
@@ -2446,8 +2523,9 @@
       <c r="J35" s="40"/>
       <c r="K35" s="9"/>
       <c r="L35" s="10"/>
-    </row>
-    <row r="36" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M35" s="44"/>
+    </row>
+    <row r="36" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A36" s="21" t="s">
         <v>100</v>
       </c>
@@ -2468,8 +2546,9 @@
       <c r="J36" s="40"/>
       <c r="K36" s="9"/>
       <c r="L36" s="10"/>
-    </row>
-    <row r="37" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M36" s="44"/>
+    </row>
+    <row r="37" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A37" s="7"/>
       <c r="B37" s="19" t="s">
         <v>102</v>
@@ -2488,8 +2567,9 @@
       <c r="J37" s="40"/>
       <c r="K37" s="9"/>
       <c r="L37" s="10"/>
-    </row>
-    <row r="38" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M37" s="44"/>
+    </row>
+    <row r="38" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A38" s="7"/>
       <c r="B38" s="19" t="s">
         <v>103</v>
@@ -2508,8 +2588,9 @@
       <c r="J38" s="40"/>
       <c r="K38" s="9"/>
       <c r="L38" s="10"/>
-    </row>
-    <row r="39" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M38" s="44"/>
+    </row>
+    <row r="39" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A39" s="7"/>
       <c r="B39" s="19" t="s">
         <v>104</v>
@@ -2528,8 +2609,9 @@
       <c r="J39" s="40"/>
       <c r="K39" s="9"/>
       <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A40" s="7"/>
       <c r="B40" s="19" t="s">
         <v>105</v>
@@ -2548,8 +2630,9 @@
       <c r="J40" s="40"/>
       <c r="K40" s="9"/>
       <c r="L40" s="10"/>
-    </row>
-    <row r="41" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M40" s="44"/>
+    </row>
+    <row r="41" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A41" s="7"/>
       <c r="B41" s="19" t="s">
         <v>106</v>
@@ -2568,8 +2651,9 @@
       <c r="J41" s="40"/>
       <c r="K41" s="9"/>
       <c r="L41" s="10"/>
-    </row>
-    <row r="42" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A42" s="7"/>
       <c r="B42" s="19" t="s">
         <v>107</v>
@@ -2588,8 +2672,9 @@
       <c r="J42" s="40"/>
       <c r="K42" s="9"/>
       <c r="L42" s="10"/>
-    </row>
-    <row r="43" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A43" s="7"/>
       <c r="B43" s="19"/>
       <c r="C43" s="8"/>
@@ -2606,8 +2691,9 @@
       <c r="J43" s="40"/>
       <c r="K43" s="9"/>
       <c r="L43" s="10"/>
-    </row>
-    <row r="44" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A44" s="7"/>
       <c r="B44" s="19" t="s">
         <v>108</v>
@@ -2626,8 +2712,9 @@
       <c r="J44" s="40"/>
       <c r="K44" s="9"/>
       <c r="L44" s="10"/>
-    </row>
-    <row r="45" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M44" s="44"/>
+    </row>
+    <row r="45" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A45" s="7"/>
       <c r="B45" s="19" t="s">
         <v>109</v>
@@ -2646,8 +2733,9 @@
       <c r="J45" s="40"/>
       <c r="K45" s="9"/>
       <c r="L45" s="10"/>
-    </row>
-    <row r="46" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M45" s="44"/>
+    </row>
+    <row r="46" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A46" s="7"/>
       <c r="B46" s="19" t="s">
         <v>110</v>
@@ -2666,8 +2754,9 @@
       <c r="J46" s="40"/>
       <c r="K46" s="9"/>
       <c r="L46" s="10"/>
-    </row>
-    <row r="47" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A47" s="7"/>
       <c r="B47" s="19" t="s">
         <v>111</v>
@@ -2686,8 +2775,9 @@
       <c r="J47" s="40"/>
       <c r="K47" s="9"/>
       <c r="L47" s="10"/>
-    </row>
-    <row r="48" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M47" s="44"/>
+    </row>
+    <row r="48" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A48" s="7"/>
       <c r="B48" s="19"/>
       <c r="C48" s="8"/>
@@ -2704,8 +2794,9 @@
       <c r="J48" s="40"/>
       <c r="K48" s="9"/>
       <c r="L48" s="10"/>
-    </row>
-    <row r="49" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M48" s="44"/>
+    </row>
+    <row r="49" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A49" s="7"/>
       <c r="B49" s="19" t="s">
         <v>112</v>
@@ -2724,8 +2815,9 @@
       <c r="J49" s="40"/>
       <c r="K49" s="9"/>
       <c r="L49" s="10"/>
-    </row>
-    <row r="50" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M49" s="44"/>
+    </row>
+    <row r="50" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A50" s="7"/>
       <c r="B50" s="19" t="s">
         <v>113</v>
@@ -2744,8 +2836,9 @@
       <c r="J50" s="40"/>
       <c r="K50" s="9"/>
       <c r="L50" s="10"/>
-    </row>
-    <row r="51" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M50" s="44"/>
+    </row>
+    <row r="51" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A51" s="7"/>
       <c r="B51" s="19" t="s">
         <v>114</v>
@@ -2764,8 +2857,9 @@
       <c r="J51" s="40"/>
       <c r="K51" s="9"/>
       <c r="L51" s="10"/>
-    </row>
-    <row r="52" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M51" s="44"/>
+    </row>
+    <row r="52" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A52" s="7"/>
       <c r="B52" s="22" t="s">
         <v>141</v>
@@ -2784,8 +2878,9 @@
       <c r="J52" s="40"/>
       <c r="K52" s="9"/>
       <c r="L52" s="10"/>
-    </row>
-    <row r="53" spans="1:12" customFormat="1" ht="45" hidden="1" customHeight="1">
+      <c r="M52" s="44"/>
+    </row>
+    <row r="53" spans="1:13" customFormat="1" ht="45" customHeight="1">
       <c r="A53" s="23"/>
       <c r="B53" s="25" t="s">
         <v>142</v>
@@ -2802,8 +2897,9 @@
       <c r="J53" s="41"/>
       <c r="K53" s="26"/>
       <c r="L53" s="27"/>
-    </row>
-    <row r="54" spans="1:12" ht="45" customHeight="1">
+      <c r="M53" s="44"/>
+    </row>
+    <row r="54" spans="1:13" ht="45" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2817,7 +2913,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="45" customHeight="1">
+    <row r="55" spans="1:13" ht="45" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2831,7 +2927,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="45" customHeight="1">
+    <row r="56" spans="1:13" ht="45" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2845,7 +2941,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="45" customHeight="1">
+    <row r="57" spans="1:13" ht="45" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2859,7 +2955,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="45" customHeight="1">
+    <row r="58" spans="1:13" ht="45" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2873,7 +2969,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="45" customHeight="1">
+    <row r="59" spans="1:13" ht="45" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2887,7 +2983,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="45" customHeight="1">
+    <row r="60" spans="1:13" ht="45" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2901,7 +2997,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="45" customHeight="1">
+    <row r="61" spans="1:13" ht="45" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2915,7 +3011,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="45" customHeight="1">
+    <row r="62" spans="1:13" ht="45" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2929,7 +3025,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="45" customHeight="1">
+    <row r="63" spans="1:13" ht="45" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2943,7 +3039,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="45" customHeight="1">
+    <row r="64" spans="1:13" ht="45" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>

</xml_diff>